<commit_message>
2025-09-20: Slight adjustment to the Excel spreadsheet.
</commit_message>
<xml_diff>
--- a/2025-09-13/HR.xlsx
+++ b/2025-09-13/HR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Desktop\Google data certificate + case studies\EDA lesson\EDA practices\Rstudio Practice\2025-09-13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AF1585-4557-46D4-BFC4-CC05F992CDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7922507E-49B6-4053-A631-AAD1347A9708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDA comparing performance score" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Appendix!$O$47:$O$59</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Appendix!$P$47:$P$59</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Appendix!$I$47:$I$289</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Appendix!$J$47:$J$289</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Appendix!$F$47:$F$83</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Appendix!$G$47:$G$83</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Appendix!$L$47:$L$64</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Appendix!$M$47:$M$64</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Appendix!$L$47:$L$64</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Appendix!$M$47:$M$64</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Appendix!$I$47:$I$289</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Appendix!$J$47:$J$289</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Appendix!$F$47:$F$83</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Appendix!$G$47:$G$83</definedName>
     <definedName name="actual">#REF!</definedName>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">Appendix!$B$10:$C$321</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Statistical Model'!$A$9:$D$320</definedName>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="118">
   <si>
     <t>PerformanceScore</t>
   </si>
@@ -694,9 +694,6 @@
     <t>Precision</t>
   </si>
   <si>
-    <t>Recall</t>
-  </si>
-  <si>
     <t>TP Rate</t>
   </si>
   <si>
@@ -705,13 +702,107 @@
   <si>
     <t>Performance Score (1 = Poor Performance)</t>
   </si>
+  <si>
+    <t>what percentage of our predicted model accurately match with actual result?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; </t>
+  </si>
+  <si>
+    <t>CONFUSION MATRIX</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Recall/Sensitivity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">what percentage of our model accurately predicted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>positive outcome (y = 1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  compared to the actual result?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">what percentage of the actual </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>positive outcome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is accurately encapsulated by our model?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(How well did our model capture </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">actual </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>positive outcome)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -866,11 +957,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -887,10 +979,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -2746,10 +2840,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2810,10 +2904,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2874,10 +2968,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -20158,856 +20252,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4C15EA5D-63D6-4FB7-9FD1-3D45AC5C3F76}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="B63:C68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="30">
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="33">
-        <item x="10"/>
-        <item x="22"/>
-        <item x="11"/>
-        <item x="17"/>
-        <item x="13"/>
-        <item x="31"/>
-        <item x="5"/>
-        <item x="30"/>
-        <item x="28"/>
-        <item x="6"/>
-        <item x="14"/>
-        <item x="21"/>
-        <item x="7"/>
-        <item x="20"/>
-        <item x="29"/>
-        <item x="26"/>
-        <item x="18"/>
-        <item x="4"/>
-        <item x="19"/>
-        <item x="23"/>
-        <item x="27"/>
-        <item x="9"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="16"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="15"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="3">
-        <item n="Male" x="0"/>
-        <item n="Female" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="7">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="19">
-        <item x="4"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="7"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="7">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="21">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="14"/>
-        <item x="16"/>
-        <item x="10"/>
-        <item x="12"/>
-        <item x="9"/>
-        <item x="18"/>
-        <item x="17"/>
-        <item x="8"/>
-        <item x="13"/>
-        <item x="15"/>
-        <item x="3"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="19"/>
-        <item x="5"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of EngagementSurvey" fld="24" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
-  </dataFields>
-  <conditionalFormats count="1">
-    <conditionalFormat priority="1">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="4" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{39CB0352-D678-4E03-9967-6ABD34299ED2}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="B8:C13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="30">
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="% of PerformanceScore" fld="3" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D79B3932-D2EA-4CE2-AB0F-484D3F162B41}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="B28:I34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="30">
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="ascending">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="33">
-        <item x="10"/>
-        <item x="22"/>
-        <item x="11"/>
-        <item x="17"/>
-        <item x="13"/>
-        <item x="31"/>
-        <item x="5"/>
-        <item x="30"/>
-        <item x="28"/>
-        <item x="6"/>
-        <item x="14"/>
-        <item x="21"/>
-        <item x="7"/>
-        <item x="20"/>
-        <item x="29"/>
-        <item x="26"/>
-        <item x="18"/>
-        <item x="4"/>
-        <item x="19"/>
-        <item x="23"/>
-        <item x="27"/>
-        <item x="9"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="16"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="15"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="3">
-        <item n="Male" x="0"/>
-        <item n="Female" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
-      <items count="7">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="19">
-        <item x="4"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="7"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="21">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="14"/>
-        <item x="16"/>
-        <item x="10"/>
-        <item x="12"/>
-        <item x="9"/>
-        <item x="18"/>
-        <item x="17"/>
-        <item x="8"/>
-        <item x="13"/>
-        <item x="15"/>
-        <item x="3"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="19"/>
-        <item x="5"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="14"/>
-  </colFields>
-  <colItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name=" " fld="3" subtotal="count" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <conditionalFormats count="3">
-    <conditionalFormat priority="9">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="2" selected="0">
-              <x v="2"/>
-              <x v="3"/>
-            </reference>
-            <reference field="14" count="6" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="10">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="14" count="6" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="11">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="4" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-            </reference>
-            <reference field="14" count="6" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6078FAE4-58D5-4E44-850A-3409EAF797D9}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="B49:F57" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="30">
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" compact="0" outline="0" showAll="0" sortType="ascending">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="33">
-        <item x="10"/>
-        <item x="22"/>
-        <item x="11"/>
-        <item x="17"/>
-        <item x="13"/>
-        <item x="31"/>
-        <item x="5"/>
-        <item x="30"/>
-        <item x="28"/>
-        <item x="6"/>
-        <item x="14"/>
-        <item x="21"/>
-        <item x="7"/>
-        <item x="20"/>
-        <item x="29"/>
-        <item x="26"/>
-        <item x="18"/>
-        <item x="4"/>
-        <item x="19"/>
-        <item x="23"/>
-        <item x="27"/>
-        <item x="9"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="16"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="15"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="3">
-        <item n="Male" x="0"/>
-        <item n="Female" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="7">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="19">
-        <item x="4"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="7"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="7">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="21">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="14"/>
-        <item x="16"/>
-        <item x="10"/>
-        <item x="12"/>
-        <item x="9"/>
-        <item x="18"/>
-        <item x="17"/>
-        <item x="8"/>
-        <item x="13"/>
-        <item x="15"/>
-        <item x="3"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="19"/>
-        <item x="5"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="20"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="3"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name=" " fld="3" subtotal="count" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <conditionalFormats count="3">
-    <conditionalFormat priority="12">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="2" selected="0">
-              <x v="2"/>
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="6" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="13">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="6" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="14">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="6" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC6F0180-D54F-48DE-8D6D-4CCA337465AA}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="B17:E23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="30">
@@ -21210,7 +20454,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A06E586F-AA5D-40DB-8861-8E10DFC14E7A}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="K8:Q14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="30">
@@ -21583,7 +20827,1036 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4C15EA5D-63D6-4FB7-9FD1-3D45AC5C3F76}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="B63:C68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="30">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="33">
+        <item x="10"/>
+        <item x="22"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="13"/>
+        <item x="31"/>
+        <item x="5"/>
+        <item x="30"/>
+        <item x="28"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item x="7"/>
+        <item x="20"/>
+        <item x="29"/>
+        <item x="26"/>
+        <item x="18"/>
+        <item x="4"/>
+        <item x="19"/>
+        <item x="23"/>
+        <item x="27"/>
+        <item x="9"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="16"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="3">
+        <item n="Male" x="0"/>
+        <item n="Female" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="7">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="19">
+        <item x="4"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="7"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="7">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="21">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="16"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="9"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item x="8"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of EngagementSurvey" fld="24" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
+  </dataFields>
+  <conditionalFormats count="1">
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="4" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{39CB0352-D678-4E03-9967-6ABD34299ED2}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="B8:C13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="30">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="% of PerformanceScore" fld="3" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D79B3932-D2EA-4CE2-AB0F-484D3F162B41}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="B28:I34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="30">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="ascending">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="33">
+        <item x="10"/>
+        <item x="22"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="13"/>
+        <item x="31"/>
+        <item x="5"/>
+        <item x="30"/>
+        <item x="28"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item x="7"/>
+        <item x="20"/>
+        <item x="29"/>
+        <item x="26"/>
+        <item x="18"/>
+        <item x="4"/>
+        <item x="19"/>
+        <item x="23"/>
+        <item x="27"/>
+        <item x="9"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="16"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="3">
+        <item n="Male" x="0"/>
+        <item n="Female" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+      <items count="7">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="19">
+        <item x="4"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="7"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="21">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="16"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="9"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item x="8"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="14"/>
+  </colFields>
+  <colItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name=" " fld="3" subtotal="count" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <conditionalFormats count="3">
+    <conditionalFormat priority="9">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="2" selected="0">
+              <x v="2"/>
+              <x v="3"/>
+            </reference>
+            <reference field="14" count="6" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="10">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="14" count="6" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="11">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="4" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+            </reference>
+            <reference field="14" count="6" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6078FAE4-58D5-4E44-850A-3409EAF797D9}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="B49:F57" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="30">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" compact="0" outline="0" showAll="0" sortType="ascending">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="33">
+        <item x="10"/>
+        <item x="22"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="13"/>
+        <item x="31"/>
+        <item x="5"/>
+        <item x="30"/>
+        <item x="28"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item x="7"/>
+        <item x="20"/>
+        <item x="29"/>
+        <item x="26"/>
+        <item x="18"/>
+        <item x="4"/>
+        <item x="19"/>
+        <item x="23"/>
+        <item x="27"/>
+        <item x="9"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="16"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="3">
+        <item n="Male" x="0"/>
+        <item n="Female" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="7">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="19">
+        <item x="4"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="7"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="7">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="21">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="16"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="9"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item x="8"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="20"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name=" " fld="3" subtotal="count" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <conditionalFormats count="3">
+    <conditionalFormat priority="12">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="2" selected="0">
+              <x v="2"/>
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="6" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="13">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="6" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="14">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="6" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85F01519-D835-46AA-8D6E-95BD284E35D6}" name="PivotTable10" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="B29:F33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="30">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" compact="0" outline="0" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField name="Reason for Termination" compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="18">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="16"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="6"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="19"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name=" " fld="3" subtotal="count" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <conditionalFormats count="3">
+    <conditionalFormat priority="3">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="19" count="2" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="19" count="2" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="2" selected="0">
+              <x v="2"/>
+              <x v="3"/>
+            </reference>
+            <reference field="19" count="2" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8D9B3C61-7ADA-461A-B3ED-976C2D27D64D}" name="PivotTable8" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="B6:F25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="30">
@@ -21828,185 +22101,6 @@
               <x v="14"/>
               <x v="15"/>
               <x v="16"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85F01519-D835-46AA-8D6E-95BD284E35D6}" name="PivotTable10" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="B29:F33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="30">
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" compact="0" outline="0" showAll="0">
-      <items count="5">
-        <item x="3"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField name="Reason for Termination" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="18">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="16"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="11"/>
-        <item x="10"/>
-        <item x="12"/>
-        <item x="6"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="19"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="3"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name=" " fld="3" subtotal="count" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <conditionalFormats count="3">
-    <conditionalFormat priority="3">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="19" count="2" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="2">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="19" count="2" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="1">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="2" selected="0">
-              <x v="2"/>
-              <x v="3"/>
-            </reference>
-            <reference field="19" count="2" selected="0">
-              <x v="0"/>
-              <x v="1"/>
             </reference>
           </references>
         </pivotArea>
@@ -23308,8 +23402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C1C546-D924-47A9-84B0-FE3BDE83BEFC}">
   <dimension ref="A1:R320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23324,7 +23418,8 @@
     <col min="9" max="9" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.140625" customWidth="1"/>
-    <col min="12" max="13" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="98.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="21" width="14.140625" customWidth="1"/>
   </cols>
@@ -23355,11 +23450,8 @@
         <f>SUM(J10:J320)</f>
         <v>-20.022805498439418</v>
       </c>
-      <c r="P1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>102</v>
+      <c r="N1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -23375,31 +23467,19 @@
       <c r="D2" s="10">
         <v>-7.8269647879355177E-3</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
+      <c r="P2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N3" t="s">
-        <v>103</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3" s="12">
-        <f>COUNTIFS(Truncated_Employee_Performance_Score__for_Data_Model[PerformanceScore],$O3,predicted,P$2)</f>
-        <v>278</v>
-      </c>
-      <c r="Q3" s="12">
-        <f>COUNTIFS(Truncated_Employee_Performance_Score__for_Data_Model[PerformanceScore],$O3,predicted,Q$2)</f>
-        <v>2</v>
-      </c>
-      <c r="R3" s="13">
-        <f>SUM(P3:Q3)</f>
-        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -23407,19 +23487,19 @@
         <v>103</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="12">
-        <f>COUNTIFS(Truncated_Employee_Performance_Score__for_Data_Model[PerformanceScore],$O4,predicted,P$2)</f>
-        <v>10</v>
+        <f>COUNTIFS(Truncated_Employee_Performance_Score__for_Data_Model[PerformanceScore],$O4,predicted,P$3)</f>
+        <v>278</v>
       </c>
       <c r="Q4" s="12">
-        <f>COUNTIFS(Truncated_Employee_Performance_Score__for_Data_Model[PerformanceScore],$O4,predicted,Q$2)</f>
-        <v>21</v>
+        <f>COUNTIFS(Truncated_Employee_Performance_Score__for_Data_Model[PerformanceScore],$O4,predicted,Q$3)</f>
+        <v>2</v>
       </c>
       <c r="R4" s="13">
         <f>SUM(P4:Q4)</f>
-        <v>31</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -23427,33 +23507,58 @@
         <f>EXP(A2)/(EXP(A2)+1)</f>
         <v>0.99996810494195298</v>
       </c>
-      <c r="O5" t="s">
+      <c r="N5" t="s">
+        <v>103</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" s="12">
+        <f>COUNTIFS(Truncated_Employee_Performance_Score__for_Data_Model[PerformanceScore],$O5,predicted,P$3)</f>
+        <v>10</v>
+      </c>
+      <c r="Q5" s="12">
+        <f>COUNTIFS(Truncated_Employee_Performance_Score__for_Data_Model[PerformanceScore],$O5,predicted,Q$3)</f>
+        <v>21</v>
+      </c>
+      <c r="R5" s="13">
+        <f>SUM(P5:Q5)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
         <v>104</v>
       </c>
-      <c r="P5" s="13">
-        <f>SUM(P3:P4)</f>
+      <c r="P6" s="13">
+        <f>SUM(P4:P5)</f>
         <v>288</v>
       </c>
-      <c r="Q5" s="13">
-        <f>SUM(Q3:Q4)</f>
+      <c r="Q6" s="13">
+        <f>SUM(Q4:Q5)</f>
         <v>23</v>
       </c>
-      <c r="R5" s="14">
-        <f>SUM(R3:R4)</f>
+      <c r="R6" s="14">
+        <f>SUM(R4:R5)</f>
         <v>311</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="P7" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M8" t="s">
         <v>110</v>
       </c>
+      <c r="N8" t="s">
+        <v>111</v>
+      </c>
       <c r="P8" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="Q8" s="16">
+        <f>(P4+Q5)/R6</f>
+        <v>0.96141479099678462</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -23487,8 +23592,18 @@
       <c r="K9" t="s">
         <v>102</v>
       </c>
+      <c r="M9" t="s">
+        <v>115</v>
+      </c>
+      <c r="N9" t="s">
+        <v>113</v>
+      </c>
       <c r="P9" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="Q9" s="16">
+        <f>Q5/Q6</f>
+        <v>0.91304347826086951</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -23528,8 +23643,18 @@
         <f>IF(H10&gt;$I$1,1,0)</f>
         <v>0</v>
       </c>
+      <c r="M10" t="s">
+        <v>116</v>
+      </c>
+      <c r="N10" t="s">
+        <v>113</v>
+      </c>
       <c r="P10" t="s">
-        <v>108</v>
+        <v>114</v>
+      </c>
+      <c r="Q10" s="16">
+        <f>Q5/R5</f>
+        <v>0.67741935483870963</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -23569,8 +23694,11 @@
         <f t="shared" ref="K11:K74" si="3">IF(H11&gt;$I$1,1,0)</f>
         <v>0</v>
       </c>
+      <c r="M11" t="s">
+        <v>117</v>
+      </c>
       <c r="P11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -23609,6 +23737,9 @@
       <c r="K12">
         <f t="shared" si="3"/>
         <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>